<commit_message>
removing integer validation from excel for price override
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/CDOReview.xlsx
+++ b/requirement/src/main/resources/templates/CDOReview.xlsx
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
+      <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,14 +671,11 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="New SLA value should be a number" sqref="AF1:AF1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="CDO Quantity Override should be number" sqref="AG1:AG1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="CDO Price Override should be number" sqref="AK1:AK1048576">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
code for email system
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/CDOReview.xlsx
+++ b/requirement/src/main/resources/templates/CDOReview.xlsx
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
+      <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,14 +671,11 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="New SLA value should be a number" sqref="AF1:AF1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="CDO Quantity Override should be number" sqref="AG1:AG1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="CDO Price Override should be number" sqref="AK1:AK1048576">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>